<commit_message>
new masterinput, create rotation_spinup
</commit_message>
<xml_diff>
--- a/Scenarios/common/Nnorm_2019.xlsx
+++ b/Scenarios/common/Nnorm_2019.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="338">
   <si>
     <t>JB 1+3</t>
   </si>
@@ -1039,9 +1039,6 @@
   </si>
   <si>
     <t>norm_JB1</t>
-  </si>
-  <si>
-    <t>JB6-6-7-7-7L_low</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1084,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10713,10 +10710,13 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -11030,8 +11030,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>338</v>
+      <c r="A9">
+        <v>101</v>
       </c>
       <c r="B9" t="s">
         <v>45</v>
@@ -11181,6 +11181,9 @@
         <f>1.14*0.079/6.25</f>
         <v>1.4409599999999998E-2</v>
       </c>
+      <c r="L12">
+        <v>1.1399999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -11217,6 +11220,9 @@
         <f>1.26*0.156/6.25</f>
         <v>3.1449600000000001E-2</v>
       </c>
+      <c r="L13">
+        <v>1.26</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -11253,6 +11259,9 @@
         <f>1.16*0.2/6.25</f>
         <v>3.712E-2</v>
       </c>
+      <c r="L14">
+        <v>1.1599999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -11289,6 +11298,9 @@
         <f>1.2*0.183/6.25</f>
         <v>3.5136000000000001E-2</v>
       </c>
+      <c r="L15">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -11325,6 +11337,9 @@
         <f>1.03*0.21/6.25</f>
         <v>3.4608E-2</v>
       </c>
+      <c r="L16">
+        <v>1.03</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -11361,7 +11376,9 @@
         <f>1.21*0.173/6.25</f>
         <v>3.3492799999999996E-2</v>
       </c>
-      <c r="L17" s="4"/>
+      <c r="L17" s="4">
+        <v>1.21</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -11398,72 +11415,84 @@
         <f>1.18*0.168/6.25</f>
         <v>3.1718400000000001E-2</v>
       </c>
+      <c r="L18">
+        <v>1.18</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>970</v>
+        <v>261</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>5800</v>
+      </c>
+      <c r="K19">
+        <v>6300</v>
+      </c>
+      <c r="L19">
+        <v>1.2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>261</v>
+        <v>970</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="C20">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>5800</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>6300</v>
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>